<commit_message>
updated NomineeDetails, constantHelper, Data.xlsx files
</commit_message>
<xml_diff>
--- a/Exide_POM/Resources/data/data.xlsx
+++ b/Exide_POM/Resources/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11340" windowHeight="4095" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11340" windowHeight="3180" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Exide" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="82">
   <si>
     <t>proposalNo</t>
   </si>
@@ -234,6 +234,36 @@
   </si>
   <si>
     <t>fatherWork</t>
+  </si>
+  <si>
+    <t>nmDOBday</t>
+  </si>
+  <si>
+    <t>nmDOBmonth</t>
+  </si>
+  <si>
+    <t>nmDOByear</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
+  <si>
+    <t>nomRelation</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>nmMaritalStatus</t>
+  </si>
+  <si>
+    <t>Married</t>
   </si>
 </sst>
 </file>
@@ -313,7 +343,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -329,6 +359,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -762,10 +793,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AK1" sqref="AK1"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AP1" sqref="AP1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -792,9 +823,13 @@
     <col min="35" max="35" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.42578125" customWidth="1"/>
+    <col min="39" max="39" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:42">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -906,12 +941,27 @@
       <c r="AK1" s="5" t="s">
         <v>71</v>
       </c>
+      <c r="AL1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AO1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AP1" s="5" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:42">
       <c r="A2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -1010,14 +1060,29 @@
       <c r="AH2" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AI2" s="9" t="s">
-        <v>69</v>
+      <c r="AI2" s="9">
+        <v>100000</v>
       </c>
       <c r="AJ2" s="6" t="s">
         <v>69</v>
       </c>
       <c r="AK2" s="8" t="s">
         <v>62</v>
+      </c>
+      <c r="AL2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM2" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN2" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all commits till 17June
</commit_message>
<xml_diff>
--- a/Exide_POM/Resources/data/data.xlsx
+++ b/Exide_POM/Resources/data/data.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
   <si>
     <t>proposalNo</t>
   </si>
@@ -251,9 +251,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>1999</t>
-  </si>
-  <si>
     <t>nomRelation</t>
   </si>
   <si>
@@ -264,6 +261,18 @@
   </si>
   <si>
     <t>Married</t>
+  </si>
+  <si>
+    <t>nomShare</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>1974</t>
+  </si>
+  <si>
+    <t>sumAssured</t>
   </si>
 </sst>
 </file>
@@ -793,10 +802,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AP1" sqref="AP1"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="AR2" sqref="AR2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -827,9 +836,10 @@
     <col min="39" max="39" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42">
+    <row r="1" spans="1:44">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -951,13 +961,19 @@
         <v>74</v>
       </c>
       <c r="AO1" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AP1" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="AQ1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR1" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:42">
+    <row r="2" spans="1:44">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1076,13 +1092,19 @@
         <v>76</v>
       </c>
       <c r="AN2" s="6" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="AO2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AP2" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="AQ2" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR2">
+        <v>500000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added proposal script for plan details
</commit_message>
<xml_diff>
--- a/Exide_POM/Resources/data/data.xlsx
+++ b/Exide_POM/Resources/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11340" windowHeight="3180" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="1125" windowWidth="11340" windowHeight="5880" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Exide" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="100">
   <si>
     <t>proposalNo</t>
   </si>
@@ -272,7 +272,52 @@
     <t>1974</t>
   </si>
   <si>
+    <t>100000</t>
+  </si>
+  <si>
     <t>sumAssured</t>
+  </si>
+  <si>
+    <t>policyTerm</t>
+  </si>
+  <si>
+    <t>FreqPayment</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>700000</t>
+  </si>
+  <si>
+    <t>PSDay</t>
+  </si>
+  <si>
+    <t>PSMonth</t>
+  </si>
+  <si>
+    <t>PSYear</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>LN000002</t>
+  </si>
+  <si>
+    <t>MedClass</t>
+  </si>
+  <si>
+    <t>Non-Medical</t>
   </si>
 </sst>
 </file>
@@ -802,10 +847,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR2"/>
+  <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AR2" sqref="AR2"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="AX2" sqref="AX2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -837,9 +882,13 @@
     <col min="40" max="40" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.42578125" customWidth="1"/>
+    <col min="45" max="45" width="10.7109375" customWidth="1"/>
+    <col min="46" max="46" width="12.7109375" customWidth="1"/>
+    <col min="50" max="50" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:50">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -970,15 +1019,33 @@
         <v>81</v>
       </c>
       <c r="AR1" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
+      </c>
+      <c r="AS1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AU1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="AV1" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AW1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AX1" s="5" t="s">
+        <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:44">
+    <row r="2" spans="1:50">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>14</v>
@@ -1076,8 +1143,8 @@
       <c r="AH2" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AI2" s="9">
-        <v>100000</v>
+      <c r="AI2" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="AJ2" s="6" t="s">
         <v>69</v>
@@ -1103,8 +1170,26 @@
       <c r="AQ2" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="AR2">
-        <v>500000</v>
+      <c r="AR2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AS2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AU2" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="AV2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="AW2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Half yearly mod
</commit_message>
<xml_diff>
--- a/Exide_POM/Resources/data/data.xlsx
+++ b/Exide_POM/Resources/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1125" windowWidth="11340" windowHeight="5880" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="1125" windowWidth="11340" windowHeight="3885" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Exide" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="145">
   <si>
     <t>proposalNo</t>
   </si>
@@ -318,6 +318,141 @@
   </si>
   <si>
     <t>Non-Medical</t>
+  </si>
+  <si>
+    <t>IndAccountNo</t>
+  </si>
+  <si>
+    <t>IndConfirmAccNo</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>AccType</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>AccHoldersName</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>IndIfscCode</t>
+  </si>
+  <si>
+    <t>HDFC0002019</t>
+  </si>
+  <si>
+    <t>DebitDate</t>
+  </si>
+  <si>
+    <t>ManDateAmount</t>
+  </si>
+  <si>
+    <t>60000</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>FreqPayHalfYearly</t>
+  </si>
+  <si>
+    <t>Half Yearly</t>
+  </si>
+  <si>
+    <t>CredCardHolder</t>
+  </si>
+  <si>
+    <t>CredCardBrand</t>
+  </si>
+  <si>
+    <t>Credit Card - Matercard</t>
+  </si>
+  <si>
+    <t>Srk</t>
+  </si>
+  <si>
+    <t>CreditCardNo</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>ExpiryYear</t>
+  </si>
+  <si>
+    <t>ExpireMonth</t>
+  </si>
+  <si>
+    <t>CardIssuer</t>
+  </si>
+  <si>
+    <t>HDFC BANK</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>PayType</t>
+  </si>
+  <si>
+    <t>BankTieUp</t>
+  </si>
+  <si>
+    <t>HDFC Bank</t>
+  </si>
+  <si>
+    <t>EnterAmount</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>3392</t>
+  </si>
+  <si>
+    <t>IncomeProofType</t>
+  </si>
+  <si>
+    <t>FinYear</t>
+  </si>
+  <si>
+    <t>2018 - 19</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Salary Slip</t>
+  </si>
+  <si>
+    <t>SmokeHab</t>
+  </si>
+  <si>
+    <t>Non Smoker</t>
   </si>
 </sst>
 </file>
@@ -847,10 +982,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX2"/>
+  <dimension ref="A1:BV2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
-      <selection activeCell="AX2" sqref="AX2"/>
+    <sheetView tabSelected="1" topLeftCell="BN1" workbookViewId="0">
+      <selection activeCell="BU2" sqref="BU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -886,9 +1021,26 @@
     <col min="45" max="45" width="10.7109375" customWidth="1"/>
     <col min="46" max="46" width="12.7109375" customWidth="1"/>
     <col min="50" max="50" width="12.5703125" customWidth="1"/>
+    <col min="51" max="51" width="14.140625" customWidth="1"/>
+    <col min="52" max="52" width="17.7109375" customWidth="1"/>
+    <col min="54" max="54" width="15.7109375" customWidth="1"/>
+    <col min="55" max="55" width="12.85546875" customWidth="1"/>
+    <col min="56" max="56" width="10.5703125" customWidth="1"/>
+    <col min="57" max="57" width="16.7109375" customWidth="1"/>
+    <col min="59" max="59" width="18" customWidth="1"/>
+    <col min="60" max="60" width="14.140625" customWidth="1"/>
+    <col min="61" max="61" width="20.7109375" customWidth="1"/>
+    <col min="62" max="62" width="13.28515625" customWidth="1"/>
+    <col min="63" max="63" width="14" customWidth="1"/>
+    <col min="64" max="64" width="10.5703125" customWidth="1"/>
+    <col min="65" max="65" width="11.5703125" customWidth="1"/>
+    <col min="69" max="69" width="11" customWidth="1"/>
+    <col min="70" max="70" width="12.5703125" customWidth="1"/>
+    <col min="71" max="71" width="16.85546875" customWidth="1"/>
+    <col min="74" max="74" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50">
+    <row r="1" spans="1:74">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -1039,8 +1191,80 @@
       <c r="AX1" s="5" t="s">
         <v>98</v>
       </c>
+      <c r="AY1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="AZ1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="BA1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="BB1" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="BC1" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="BD1" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="BE1" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="BF1" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="BG1" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="BH1" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="BI1" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="BJ1" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="BK1" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="BL1" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="BM1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="BN1" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="BO1" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="BP1" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="BQ1" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="BR1" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="BS1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="BT1" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="BU1" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="BV1" s="5" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="2" spans="1:50">
+    <row r="2" spans="1:74">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1190,6 +1414,78 @@
       </c>
       <c r="AX2" t="s">
         <v>99</v>
+      </c>
+      <c r="AY2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="AZ2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>104</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>106</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>108</v>
+      </c>
+      <c r="BD2" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="BE2" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>114</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>116</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>120</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>119</v>
+      </c>
+      <c r="BJ2">
+        <v>123456789</v>
+      </c>
+      <c r="BK2" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="BL2">
+        <v>2019</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>126</v>
+      </c>
+      <c r="BN2" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="BO2" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>131</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>134</v>
+      </c>
+      <c r="BR2" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>142</v>
+      </c>
+      <c r="BT2" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="BU2" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
monthlt, yearly and half yearly extent reports
</commit_message>
<xml_diff>
--- a/Exide_POM/Resources/data/data.xlsx
+++ b/Exide_POM/Resources/data/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1125" windowWidth="11340" windowHeight="3975" tabRatio="928" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="1125" windowWidth="11340" windowHeight="4425" tabRatio="928" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Exide" sheetId="2" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="PFMonthly" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K11"/>
+  <oleSize ref="A1:K13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="200">
   <si>
     <t>proposalNo</t>
   </si>
@@ -595,14 +595,41 @@
     <t>Master-M</t>
   </si>
   <si>
-    <t>LN000009</t>
+    <t>pan</t>
+  </si>
+  <si>
+    <t>AWXPV9306M</t>
+  </si>
+  <si>
+    <t>caseNo</t>
+  </si>
+  <si>
+    <t>targetGroupName</t>
+  </si>
+  <si>
+    <t>Valid Data</t>
+  </si>
+  <si>
+    <t>PI000022</t>
+  </si>
+  <si>
+    <t>PI000023</t>
+  </si>
+  <si>
+    <t>PI000024</t>
+  </si>
+  <si>
+    <t>InValid Data</t>
+  </si>
+  <si>
+    <t>LN000014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -682,6 +709,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF242729"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -706,7 +740,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -787,6 +821,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2982,369 +3019,391 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF2"/>
+  <dimension ref="A1:BI2"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AN1" sqref="AN1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="11"/>
+    <col min="10" max="10" width="9.140625" style="11"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:58">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:61">
+      <c r="A1" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="H1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="I1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="J1" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="K1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="L1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="M1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="N1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="O1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="P1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="Q1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="R1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="S1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="T1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="U1" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="V1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="T1" s="18" t="s">
+      <c r="W1" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="X1" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="V1" s="18" t="s">
+      <c r="Y1" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="W1" s="18" t="s">
+      <c r="Z1" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="18" t="s">
+      <c r="AA1" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="AB1" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="Z1" s="18" t="s">
+      <c r="AC1" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AA1" s="18" t="s">
+      <c r="AD1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="AB1" s="18" t="s">
+      <c r="AE1" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="AC1" s="18" t="s">
+      <c r="AF1" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="AD1" s="18" t="s">
+      <c r="AG1" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="AE1" s="18" t="s">
+      <c r="AH1" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="AF1" s="18" t="s">
+      <c r="AI1" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="AG1" s="18" t="s">
+      <c r="AJ1" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="AH1" s="18" t="s">
+      <c r="AK1" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="AI1" s="18" t="s">
+      <c r="AL1" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AJ1" s="18" t="s">
+      <c r="AM1" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="AK1" s="18" t="s">
+      <c r="AN1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="AL1" s="18" t="s">
+      <c r="AO1" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="AM1" s="18" t="s">
+      <c r="AP1" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="AN1" s="18" t="s">
+      <c r="AQ1" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="AO1" s="18" t="s">
+      <c r="AR1" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="AP1" s="18" t="s">
+      <c r="AS1" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="AQ1" s="18" t="s">
+      <c r="AT1" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="AR1" s="18" t="s">
+      <c r="AU1" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="AS1" s="18" t="s">
+      <c r="AV1" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="AT1" s="18" t="s">
+      <c r="AW1" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="AU1" s="18" t="s">
+      <c r="AX1" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="AV1" s="18" t="s">
+      <c r="AY1" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="AW1" s="18" t="s">
+      <c r="AZ1" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="AX1" s="18" t="s">
+      <c r="BA1" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="AY1" s="18" t="s">
+      <c r="BB1" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="AZ1" s="18" t="s">
+      <c r="BC1" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="BA1" s="18" t="s">
+      <c r="BD1" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="BB1" s="18" t="s">
+      <c r="BE1" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="BC1" s="18" t="s">
+      <c r="BF1" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="BD1" s="18" t="s">
+      <c r="BG1" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="BE1" s="18" t="s">
+      <c r="BH1" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="BF1" s="18" t="s">
+      <c r="BI1" s="18" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:58">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:61">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="C2" s="21" t="s">
+      <c r="D2" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="F2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="G2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="H2" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="I2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="J2" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="K2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="L2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="M2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="N2" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="O2" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="P2" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="Q2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="22" t="s">
+      <c r="R2" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="22" t="s">
+      <c r="S2" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="22" t="s">
+      <c r="T2" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="17" t="s">
+      <c r="U2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="17" t="s">
+      <c r="V2" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="T2" s="22" t="s">
+      <c r="W2" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="22" t="s">
+      <c r="X2" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="22" t="s">
+      <c r="Y2" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="W2" s="22" t="s">
+      <c r="Z2" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="X2" s="24" t="s">
+      <c r="AA2" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="Y2" s="22" t="s">
+      <c r="AB2" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="Z2" s="24" t="s">
+      <c r="AC2" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="AA2" s="23" t="s">
+      <c r="AD2" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="AB2" s="22" t="s">
+      <c r="AE2" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="AC2" s="22" t="s">
+      <c r="AF2" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="AD2" s="22" t="s">
+      <c r="AG2" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="AE2" s="22" t="s">
+      <c r="AH2" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="AF2" s="22" t="s">
+      <c r="AI2" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="AG2" s="25" t="s">
+      <c r="AJ2" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="AH2" s="17" t="s">
+      <c r="AK2" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="AI2" s="17" t="s">
+      <c r="AL2" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="AJ2" s="24" t="s">
+      <c r="AM2" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="AK2" s="24" t="s">
+      <c r="AN2" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="AL2" s="22" t="s">
+      <c r="AO2" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="AM2" s="24" t="s">
+      <c r="AP2" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="AN2" s="52" t="s">
+      <c r="AQ2" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="AO2" s="17">
+      <c r="AR2" s="17">
         <v>1974</v>
       </c>
-      <c r="AP2" s="17" t="s">
+      <c r="AS2" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="AQ2" s="17" t="s">
+      <c r="AT2" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="AR2" s="24" t="s">
+      <c r="AU2" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="AS2" s="24" t="s">
+      <c r="AV2" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="AT2" s="24" t="s">
+      <c r="AW2" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="AU2" s="17" t="s">
+      <c r="AX2" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="AV2" s="24" t="s">
+      <c r="AY2" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="AW2" s="24" t="s">
+      <c r="AZ2" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="AX2" s="24" t="s">
+      <c r="BA2" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="AY2" s="17" t="s">
+      <c r="BB2" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="AZ2" s="17" t="s">
+      <c r="BC2" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="BA2" s="24" t="s">
+      <c r="BD2" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="BB2" s="24" t="s">
+      <c r="BE2" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="BC2" s="17" t="s">
+      <c r="BF2" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="BD2" s="17" t="s">
+      <c r="BG2" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="BE2" s="17" t="s">
+      <c r="BH2" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="BF2" s="24" t="s">
+      <c r="BI2" s="24" t="s">
         <v>135</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AA2" r:id="rId1"/>
+    <hyperlink ref="AD2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3352,426 +3411,446 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BN2"/>
+  <dimension ref="A1:BQ2"/>
   <sheetViews>
-    <sheetView topLeftCell="BI1" workbookViewId="0">
-      <selection activeCell="BO3" sqref="BO3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="56" max="56" width="11.85546875" customWidth="1"/>
-    <col min="58" max="58" width="15.7109375" customWidth="1"/>
-    <col min="59" max="59" width="14" customWidth="1"/>
-    <col min="60" max="60" width="15.7109375" customWidth="1"/>
-    <col min="61" max="61" width="15.28515625" customWidth="1"/>
-    <col min="62" max="62" width="16.85546875" customWidth="1"/>
-    <col min="63" max="64" width="17.85546875" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="11"/>
+    <col min="10" max="10" width="9.140625" style="11"/>
+    <col min="59" max="59" width="11.85546875" customWidth="1"/>
+    <col min="61" max="61" width="15.7109375" customWidth="1"/>
+    <col min="62" max="62" width="14" customWidth="1"/>
+    <col min="63" max="63" width="15.7109375" customWidth="1"/>
+    <col min="64" max="64" width="15.28515625" customWidth="1"/>
+    <col min="65" max="65" width="16.85546875" customWidth="1"/>
+    <col min="66" max="67" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:69">
+      <c r="A1" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="D1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="E1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="F1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="G1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="H1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="I1" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="J1" s="47" t="s">
+        <v>190</v>
+      </c>
+      <c r="K1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="L1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="M1" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="N1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="O1" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="P1" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="Q1" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="R1" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="S1" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="T1" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="U1" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="V1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="W1" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="X1" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="Y1" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="Z1" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="AA1" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="Y1" s="27" t="s">
+      <c r="AB1" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="Z1" s="27" t="s">
+      <c r="AC1" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="AA1" s="27" t="s">
+      <c r="AD1" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="AB1" s="27" t="s">
+      <c r="AE1" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="AC1" s="27" t="s">
+      <c r="AF1" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="AD1" s="27" t="s">
+      <c r="AG1" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="AE1" s="27" t="s">
+      <c r="AH1" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="AF1" s="27" t="s">
+      <c r="AI1" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="AG1" s="27" t="s">
+      <c r="AJ1" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="AH1" s="27" t="s">
+      <c r="AK1" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="AI1" s="27" t="s">
+      <c r="AL1" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="AJ1" s="27" t="s">
+      <c r="AM1" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="AK1" s="27" t="s">
+      <c r="AN1" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="AL1" s="27" t="s">
+      <c r="AO1" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="AM1" s="27" t="s">
+      <c r="AP1" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="AN1" s="27" t="s">
+      <c r="AQ1" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="AO1" s="27" t="s">
+      <c r="AR1" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="AP1" s="27" t="s">
+      <c r="AS1" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="AQ1" s="27" t="s">
+      <c r="AT1" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="AR1" s="27" t="s">
+      <c r="AU1" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="AS1" s="27" t="s">
+      <c r="AV1" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="AT1" s="27" t="s">
+      <c r="AW1" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="AU1" s="27" t="s">
+      <c r="AX1" s="27" t="s">
         <v>163</v>
       </c>
-      <c r="AV1" s="27" t="s">
+      <c r="AY1" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="AW1" s="27" t="s">
+      <c r="AZ1" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="AX1" s="27" t="s">
+      <c r="BA1" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="AY1" s="27" t="s">
+      <c r="BB1" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="AZ1" s="27" t="s">
+      <c r="BC1" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="BA1" s="27" t="s">
+      <c r="BD1" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="BB1" s="27" t="s">
+      <c r="BE1" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="BC1" s="27" t="s">
+      <c r="BF1" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="BD1" s="27" t="s">
+      <c r="BG1" s="27" t="s">
         <v>166</v>
       </c>
-      <c r="BE1" s="27" t="s">
+      <c r="BH1" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="BF1" s="12" t="s">
+      <c r="BI1" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="BG1" s="14" t="s">
+      <c r="BJ1" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="BH1" s="14" t="s">
+      <c r="BK1" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="BI1" s="14" t="s">
+      <c r="BL1" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="BJ1" s="14" t="s">
+      <c r="BM1" s="14" t="s">
         <v>179</v>
       </c>
-      <c r="BK1" s="14" t="s">
+      <c r="BN1" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="BL1" s="14" t="s">
+      <c r="BO1" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="BM1" s="14" t="s">
+      <c r="BP1" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="BN1" s="14" t="s">
+      <c r="BQ1" s="14" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:66">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:69">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="D2" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="E2" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="F2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="G2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="H2" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="I2" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="J2" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="K2" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="L2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="M2" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="N2" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="O2" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="31" t="s">
+      <c r="P2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="34" t="s">
+      <c r="Q2" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="31" t="s">
+      <c r="R2" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="31" t="s">
+      <c r="S2" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="31" t="s">
+      <c r="T2" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="U2" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="26" t="s">
+      <c r="V2" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="T2" s="31" t="s">
+      <c r="W2" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="31" t="s">
+      <c r="X2" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="31" t="s">
+      <c r="Y2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="W2" s="31" t="s">
+      <c r="Z2" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="X2" s="33" t="s">
+      <c r="AA2" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="Y2" s="31" t="s">
+      <c r="AB2" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="Z2" s="33" t="s">
+      <c r="AC2" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="AA2" s="32" t="s">
+      <c r="AD2" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="AB2" s="31" t="s">
+      <c r="AE2" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="AC2" s="31" t="s">
+      <c r="AF2" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="AD2" s="31" t="s">
+      <c r="AG2" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="AE2" s="31" t="s">
+      <c r="AH2" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="AF2" s="31" t="s">
+      <c r="AI2" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="AG2" s="34" t="s">
+      <c r="AJ2" s="34" t="s">
         <v>83</v>
       </c>
-      <c r="AH2" s="26" t="s">
+      <c r="AK2" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="AI2" s="26" t="s">
+      <c r="AL2" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="AJ2" s="33" t="s">
+      <c r="AM2" s="33" t="s">
         <v>134</v>
       </c>
-      <c r="AK2" s="33" t="s">
+      <c r="AN2" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="AL2" s="31" t="s">
+      <c r="AO2" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="AM2" s="33" t="s">
+      <c r="AP2" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="AN2" s="52" t="s">
+      <c r="AQ2" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="AO2" s="52" t="s">
+      <c r="AR2" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="AP2" s="26" t="s">
+      <c r="AS2" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="AQ2" s="26" t="s">
+      <c r="AT2" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="AR2" s="33" t="s">
+      <c r="AU2" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="AS2" s="33" t="s">
+      <c r="AV2" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="AT2" s="33" t="s">
+      <c r="AW2" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="AU2" s="26" t="s">
+      <c r="AX2" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="AV2" s="33" t="s">
+      <c r="AY2" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="AW2" s="33" t="s">
+      <c r="AZ2" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="AX2" s="33" t="s">
+      <c r="BA2" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="AY2" s="26" t="s">
+      <c r="BB2" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="AZ2" s="26" t="s">
+      <c r="BC2" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="BA2" s="33" t="s">
+      <c r="BD2" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="BB2" s="33" t="s">
+      <c r="BE2" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="BC2" s="26" t="s">
+      <c r="BF2" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="BD2" s="26" t="s">
+      <c r="BG2" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="BE2" s="26" t="s">
+      <c r="BH2" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="BF2" s="56" t="s">
+      <c r="BI2" s="56" t="s">
         <v>189</v>
       </c>
-      <c r="BG2" s="55" t="s">
+      <c r="BJ2" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="BH2" s="55" t="s">
+      <c r="BK2" s="55" t="s">
         <v>184</v>
       </c>
-      <c r="BI2" s="55" t="s">
+      <c r="BL2" s="55" t="s">
         <v>185</v>
       </c>
-      <c r="BJ2" s="55" t="s">
+      <c r="BM2" s="55" t="s">
         <v>186</v>
       </c>
-      <c r="BK2" s="15" t="s">
+      <c r="BN2" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="BL2" s="57" t="s">
+      <c r="BO2" s="57" t="s">
         <v>162</v>
       </c>
-      <c r="BM2" s="15" t="s">
+      <c r="BP2" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="BN2" s="15" t="s">
+      <c r="BQ2" s="15" t="s">
         <v>187</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AA2" r:id="rId1"/>
+    <hyperlink ref="AD2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -3780,548 +3859,1118 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CJ2"/>
+  <dimension ref="A1:CN4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="82" max="82" width="17.28515625" style="11" customWidth="1"/>
-    <col min="88" max="88" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="11"/>
+    <col min="2" max="2" width="16.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="11"/>
+    <col min="68" max="68" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="17.28515625" style="11" customWidth="1"/>
+    <col min="91" max="91" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:92">
+      <c r="A1" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="D1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="E1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="F1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="G1" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="H1" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="I1" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="J1" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="K1" s="50" t="s">
+        <v>190</v>
+      </c>
+      <c r="L1" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="M1" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="N1" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="O1" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="P1" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="50" t="s">
+      <c r="Q1" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="50" t="s">
+      <c r="R1" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="P1" s="50" t="s">
+      <c r="S1" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="50" t="s">
+      <c r="T1" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="50" t="s">
+      <c r="U1" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="50" t="s">
+      <c r="V1" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="50" t="s">
+      <c r="W1" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="50" t="s">
+      <c r="X1" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="V1" s="50" t="s">
+      <c r="Y1" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="50" t="s">
+      <c r="Z1" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="X1" s="50" t="s">
+      <c r="AA1" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="Y1" s="50" t="s">
+      <c r="AB1" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="Z1" s="50" t="s">
+      <c r="AC1" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="AA1" s="50" t="s">
+      <c r="AD1" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="AB1" s="50" t="s">
+      <c r="AE1" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="AC1" s="50" t="s">
+      <c r="AF1" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="AD1" s="50" t="s">
+      <c r="AG1" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="AE1" s="50" t="s">
+      <c r="AH1" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="AF1" s="50" t="s">
+      <c r="AI1" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="AG1" s="50" t="s">
+      <c r="AJ1" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="AH1" s="50" t="s">
+      <c r="AK1" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="AI1" s="50" t="s">
+      <c r="AL1" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="AJ1" s="50" t="s">
+      <c r="AM1" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="AK1" s="50" t="s">
+      <c r="AN1" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="AL1" s="50" t="s">
+      <c r="AO1" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="AM1" s="50" t="s">
+      <c r="AP1" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="AN1" s="50" t="s">
+      <c r="AQ1" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="AO1" s="50" t="s">
+      <c r="AR1" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="AP1" s="50" t="s">
+      <c r="AS1" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="AQ1" s="50" t="s">
+      <c r="AT1" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="AR1" s="50" t="s">
+      <c r="AU1" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="AS1" s="50" t="s">
+      <c r="AV1" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="AT1" s="50" t="s">
+      <c r="AW1" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="AU1" s="50" t="s">
+      <c r="AX1" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="AV1" s="50" t="s">
+      <c r="AY1" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="AW1" s="50" t="s">
+      <c r="AZ1" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="AX1" s="50" t="s">
+      <c r="BA1" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="AY1" s="50" t="s">
+      <c r="BB1" s="50" t="s">
         <v>98</v>
       </c>
-      <c r="AZ1" s="50" t="s">
+      <c r="BC1" s="50" t="s">
         <v>99</v>
       </c>
-      <c r="BA1" s="50" t="s">
+      <c r="BD1" s="50" t="s">
         <v>101</v>
       </c>
-      <c r="BB1" s="50" t="s">
+      <c r="BE1" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="BC1" s="50" t="s">
+      <c r="BF1" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="BD1" s="50" t="s">
+      <c r="BG1" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="BE1" s="50" t="s">
+      <c r="BH1" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="BF1" s="50" t="s">
+      <c r="BI1" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="BG1" s="50" t="s">
+      <c r="BJ1" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="BH1" s="50" t="s">
+      <c r="BK1" s="50" t="s">
         <v>115</v>
       </c>
-      <c r="BI1" s="50" t="s">
+      <c r="BL1" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="BJ1" s="50" t="s">
+      <c r="BM1" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="BK1" s="50" t="s">
+      <c r="BN1" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="BL1" s="50" t="s">
+      <c r="BO1" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="BM1" s="50" t="s">
+      <c r="BP1" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="BN1" s="50" t="s">
+      <c r="BQ1" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="BO1" s="50" t="s">
+      <c r="BR1" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="BP1" s="50" t="s">
+      <c r="BS1" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="BQ1" s="50" t="s">
+      <c r="BT1" s="50" t="s">
         <v>131</v>
       </c>
-      <c r="BR1" s="50" t="s">
+      <c r="BU1" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="BS1" s="50" t="s">
+      <c r="BV1" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="BT1" s="50" t="s">
+      <c r="BW1" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="BU1" s="50" t="s">
+      <c r="BX1" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="BV1" s="50" t="s">
+      <c r="BY1" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="BW1" s="50" t="s">
+      <c r="BZ1" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="BX1" s="50" t="s">
+      <c r="CA1" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="BY1" s="50" t="s">
+      <c r="CB1" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="BZ1" s="50" t="s">
+      <c r="CC1" s="50" t="s">
         <v>149</v>
       </c>
-      <c r="CA1" s="50" t="s">
+      <c r="CD1" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="CB1" s="50" t="s">
+      <c r="CE1" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="CC1" s="50" t="s">
+      <c r="CF1" s="50" t="s">
         <v>152</v>
       </c>
-      <c r="CD1" s="50" t="s">
+      <c r="CG1" s="50" t="s">
         <v>168</v>
       </c>
-      <c r="CE1" s="50" t="s">
+      <c r="CH1" s="50" t="s">
         <v>155</v>
       </c>
-      <c r="CF1" s="50" t="s">
+      <c r="CI1" s="50" t="s">
         <v>156</v>
       </c>
-      <c r="CG1" s="50" t="s">
+      <c r="CJ1" s="50" t="s">
         <v>158</v>
       </c>
-      <c r="CH1" s="50" t="s">
+      <c r="CK1" s="50" t="s">
         <v>161</v>
       </c>
-      <c r="CI1" s="50" t="s">
+      <c r="CL1" s="50" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:88">
-      <c r="A2" s="45" t="s">
+    <row r="2" spans="1:92" customFormat="1">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="48" t="s">
-        <v>190</v>
-      </c>
-      <c r="C2" s="53" t="s">
+      <c r="D2" s="48" t="s">
+        <v>195</v>
+      </c>
+      <c r="E2" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="F2" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="G2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="H2" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="I2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="52" t="s">
+      <c r="J2" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="49" t="s">
+      <c r="K2" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="L2" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="49" t="s">
+      <c r="M2" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="K2" s="45" t="s">
+      <c r="N2" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="45" t="s">
+      <c r="O2" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="M2" s="45" t="s">
+      <c r="P2" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="49" t="s">
+      <c r="Q2" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="54" t="s">
+      <c r="R2" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="49" t="s">
+      <c r="S2" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="49" t="s">
+      <c r="T2" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="49" t="s">
+      <c r="U2" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="S2" s="49" t="s">
+      <c r="V2" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="49" t="s">
+      <c r="W2" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="U2" s="49" t="s">
+      <c r="X2" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="V2" s="49" t="s">
+      <c r="Y2" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="W2" s="49" t="s">
+      <c r="Z2" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="49" t="s">
+      <c r="AA2" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="Y2" s="49" t="s">
+      <c r="AB2" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="Z2" s="52" t="s">
+      <c r="AC2" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="AA2" s="49" t="s">
+      <c r="AD2" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="AB2" s="52" t="s">
+      <c r="AE2" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="AC2" s="51" t="s">
+      <c r="AF2" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="AD2" s="49" t="s">
+      <c r="AG2" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="AE2" s="49" t="s">
+      <c r="AH2" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="AF2" s="49" t="s">
+      <c r="AI2" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="AG2" s="49" t="s">
+      <c r="AJ2" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="AH2" s="49" t="s">
+      <c r="AK2" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="AI2" s="54" t="s">
+      <c r="AL2" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="AJ2" s="52" t="s">
+      <c r="AM2" s="52" t="s">
         <v>68</v>
       </c>
-      <c r="AK2" s="49" t="s">
+      <c r="AN2" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="AL2" s="52" t="s">
+      <c r="AO2" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="AM2" s="52" t="s">
+      <c r="AP2" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="AN2" s="52" t="s">
+      <c r="AQ2" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="AO2" s="45" t="s">
+      <c r="AR2" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="AP2" s="45" t="s">
+      <c r="AS2" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="AQ2" s="52" t="s">
+      <c r="AT2" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="AR2" s="52" t="s">
+      <c r="AU2" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="AS2" s="52" t="s">
+      <c r="AV2" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="AT2" s="45" t="s">
+      <c r="AW2" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="AU2" s="52" t="s">
+      <c r="AX2" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="AV2" s="52" t="s">
+      <c r="AY2" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="AW2" s="52" t="s">
+      <c r="AZ2" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="AX2" s="45" t="s">
+      <c r="BA2" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="AY2" s="52" t="s">
+      <c r="BB2" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="AZ2" s="52" t="s">
+      <c r="BC2" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="BA2" s="45" t="s">
+      <c r="BD2" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="BB2" s="45" t="s">
+      <c r="BE2" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="BC2" s="45" t="s">
+      <c r="BF2" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="BD2" s="52" t="s">
+      <c r="BG2" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="BE2" s="52" t="s">
+      <c r="BH2" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="BF2" s="45" t="s">
+      <c r="BI2" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="BG2" s="45" t="s">
+      <c r="BJ2" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="BH2" s="45" t="s">
+      <c r="BK2" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="BI2" s="45" t="s">
+      <c r="BL2" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="BJ2" s="45">
+      <c r="BM2" s="45">
         <v>123456789</v>
       </c>
-      <c r="BK2" s="52" t="s">
+      <c r="BN2" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="BL2" s="45">
+      <c r="BO2" s="45">
         <v>2019</v>
       </c>
-      <c r="BM2" s="45" t="s">
+      <c r="BP2" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="BN2" s="52" t="s">
+      <c r="BQ2" s="52" t="s">
         <v>126</v>
       </c>
-      <c r="BO2" s="52" t="s">
+      <c r="BR2" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="BP2" s="45" t="s">
+      <c r="BS2" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="BQ2" s="45" t="s">
+      <c r="BT2" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="BR2" s="52" t="s">
+      <c r="BU2" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="BS2" s="45" t="s">
+      <c r="BV2" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="BT2" s="52" t="s">
+      <c r="BW2" s="52" t="s">
         <v>138</v>
       </c>
-      <c r="BU2" s="52" t="s">
+      <c r="BX2" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="BV2" s="45" t="s">
+      <c r="BY2" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="BW2" s="45" t="s">
+      <c r="BZ2" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="BX2" s="45" t="s">
+      <c r="CA2" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="BY2" s="45">
+      <c r="CB2" s="45">
         <v>123456</v>
       </c>
-      <c r="BZ2" s="45">
+      <c r="CC2" s="45">
         <v>2000</v>
       </c>
-      <c r="CA2" s="52" t="s">
+      <c r="CD2" s="52" t="s">
         <v>153</v>
       </c>
-      <c r="CB2" s="52" t="s">
+      <c r="CE2" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="CC2" s="45">
+      <c r="CF2" s="45">
         <v>2019</v>
       </c>
-      <c r="CD2" s="45" t="s">
+      <c r="CG2" s="45" t="s">
         <v>169</v>
       </c>
-      <c r="CE2" s="45" t="s">
+      <c r="CH2" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="CF2" s="45" t="s">
+      <c r="CI2" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="CG2" s="52" t="s">
+      <c r="CJ2" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="CH2" s="52" t="s">
+      <c r="CK2" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="CI2" s="45" t="s">
+      <c r="CL2" s="45" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:92" s="11" customFormat="1">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>196</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="L3" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="S3" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="U3" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="V3" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="W3" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="X3" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z3" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA3" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB3" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC3" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD3" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE3" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF3" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG3" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH3" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI3" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ3" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK3" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL3" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM3" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN3" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO3" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP3" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ3" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR3" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS3" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT3" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="AU3" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="AV3" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="AW3" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="AX3" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="AY3" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="AZ3" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA3" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="BB3" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="BC3" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="BD3" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="BE3" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="BF3" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="BG3" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="BH3" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="BI3" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="BJ3" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="BK3" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="BL3" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="BM3" s="45">
+        <v>123456789</v>
+      </c>
+      <c r="BN3" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="BO3" s="45">
+        <v>2019</v>
+      </c>
+      <c r="BP3" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="BQ3" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="BR3" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="BS3" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="BT3" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="BU3" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="BV3" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="BW3" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="BX3" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="BY3" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="BZ3" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="CA3" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="CB3" s="45">
+        <v>123456</v>
+      </c>
+      <c r="CC3" s="45">
+        <v>2000</v>
+      </c>
+      <c r="CD3" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="CE3" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="CF3" s="45">
+        <v>2019</v>
+      </c>
+      <c r="CG3" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="CH3" s="45" t="s">
+        <v>162</v>
+      </c>
+      <c r="CI3" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="CJ3" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="CK3" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="CL3" s="45" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:92" s="11" customFormat="1">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="L4" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="S4" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="U4" s="49" t="s">
+        <v>36</v>
+      </c>
+      <c r="V4" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="W4" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="X4" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y4" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z4" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA4" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB4" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC4" s="52" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD4" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE4" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF4" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG4" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="AH4" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI4" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ4" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK4" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL4" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM4" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="AN4" s="49" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO4" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP4" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ4" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR4" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS4" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT4" s="52" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU4" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="AV4" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="AW4" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="AX4" s="52" t="s">
+        <v>93</v>
+      </c>
+      <c r="AY4" s="52" t="s">
+        <v>94</v>
+      </c>
+      <c r="AZ4" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA4" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="BB4" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="BC4" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="BD4" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="BE4" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="BF4" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="BG4" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="BH4" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="BI4" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="BJ4" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="BK4" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="BL4" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="BM4" s="45">
+        <v>123456789</v>
+      </c>
+      <c r="BN4" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="BO4" s="45">
+        <v>2019</v>
+      </c>
+      <c r="BP4" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="BQ4" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="BR4" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="BS4" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="BT4" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="BU4" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="BV4" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="BW4" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="BX4" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="BY4" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="BZ4" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="CA4" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="CB4" s="45">
+        <v>123456</v>
+      </c>
+      <c r="CC4" s="45">
+        <v>2000</v>
+      </c>
+      <c r="CD4" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="CE4" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="CF4" s="45">
+        <v>2019</v>
+      </c>
+      <c r="CG4" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="CH4" s="45" t="s">
+        <v>162</v>
+      </c>
+      <c r="CI4" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="CJ4" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="CK4" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="CL4" s="45" t="s">
         <v>160</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AC2" r:id="rId1"/>
+    <hyperlink ref="AF2" r:id="rId1"/>
+    <hyperlink ref="AF3" r:id="rId2"/>
+    <hyperlink ref="AF4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>